<commit_message>
Update schematics VCU et ajout protocoles de tests
Ajout de protocoles de tests et ajout de l'interface microSD dans les schematics
</commit_message>
<xml_diff>
--- a/VCU/VCU/Table de composants.xlsx
+++ b/VCU/VCU/Table de composants.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="22">
   <si>
     <t xml:space="preserve">Composant</t>
   </si>
@@ -32,12 +32,18 @@
     <t xml:space="preserve">Datasheet</t>
   </si>
   <si>
+    <t xml:space="preserve">mathieu.astagneau@etu.ec-lyon.fr</t>
+  </si>
+  <si>
     <t xml:space="preserve">Microcontrôleur</t>
   </si>
   <si>
     <t xml:space="preserve">ATSAMC21J18A-ANT</t>
   </si>
   <si>
+    <t xml:space="preserve">8vr91L2xhmMpjdtA5ubI</t>
+  </si>
+  <si>
     <t xml:space="preserve">Transceiver CAN</t>
   </si>
   <si>
@@ -60,6 +66,18 @@
   </si>
   <si>
     <t xml:space="preserve">171856-1008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Connecteur Carte microSD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DM3D-SF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Convertisseur logique 5V-3,3V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SN74LV1T34DCKRG4</t>
   </si>
   <si>
     <t xml:space="preserve">PIN VCU</t>
@@ -150,12 +168,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -180,10 +202,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I37" activeCellId="0" sqref="I37"/>
+      <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11:E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -191,6 +213,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="37.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="23.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="9.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="37.83"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -203,74 +226,107 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="F1" s="2" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>2</v>
+      <c r="B2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="ATSAMC21J18A-ANT"/>
-    <hyperlink ref="C2" r:id="rId2" display="Datasheet"/>
-    <hyperlink ref="B3" r:id="rId3" display="ATA6561-GAQW-N"/>
-    <hyperlink ref="C3" r:id="rId4" display="Datasheet"/>
-    <hyperlink ref="B4" r:id="rId5" display="TEN 40-1211E "/>
-    <hyperlink ref="C4" r:id="rId6" display="Datasheet"/>
-    <hyperlink ref="B5" r:id="rId7" display="PG164150"/>
-    <hyperlink ref="C5" r:id="rId8" display="Datasheet"/>
-    <hyperlink ref="B6" r:id="rId9" display="171856-1008"/>
-    <hyperlink ref="C6" r:id="rId10" display="Datasheet"/>
+    <hyperlink ref="F1" r:id="rId1" display="mathieu.astagneau@etu.ec-lyon.fr"/>
+    <hyperlink ref="B2" r:id="rId2" display="ATSAMC21J18A-ANT"/>
+    <hyperlink ref="C2" r:id="rId3" display="Datasheet"/>
+    <hyperlink ref="B3" r:id="rId4" display="ATA6561-GAQW-N"/>
+    <hyperlink ref="C3" r:id="rId5" display="Datasheet"/>
+    <hyperlink ref="B4" r:id="rId6" display="TEN 40-1211E "/>
+    <hyperlink ref="C4" r:id="rId7" display="Datasheet"/>
+    <hyperlink ref="B5" r:id="rId8" display="PG164150"/>
+    <hyperlink ref="C5" r:id="rId9" display="Datasheet"/>
+    <hyperlink ref="B6" r:id="rId10" display="171856-1008"/>
+    <hyperlink ref="C6" r:id="rId11" display="Datasheet"/>
+    <hyperlink ref="B7" r:id="rId12" display="DM3D-SF"/>
+    <hyperlink ref="C7" r:id="rId13" display="Datasheet"/>
+    <hyperlink ref="B8" r:id="rId14" display="SN74LV1T34DCKRG4"/>
+    <hyperlink ref="C8" r:id="rId15" display="Datasheet"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -290,7 +346,7 @@
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="1" sqref="E11:E12 C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -300,13 +356,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ajout readME et Update schematics
</commit_message>
<xml_diff>
--- a/VCU/VCU/Table de composants.xlsx
+++ b/VCU/VCU/Table de composants.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
   <si>
     <t xml:space="preserve">Composant</t>
   </si>
@@ -77,7 +77,13 @@
     <t xml:space="preserve">Convertisseur logique 5V-3,3V</t>
   </si>
   <si>
-    <t xml:space="preserve">SN74LV1T34DCKRG4</t>
+    <t xml:space="preserve">TBA-1-0510</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Level shifter 5V-3,3V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CD4504BEE4</t>
   </si>
   <si>
     <t xml:space="preserve">PIN VCU</t>
@@ -177,11 +183,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -202,10 +208,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11:E12"/>
+      <selection pane="topLeft" activeCell="B11" activeCellId="1" sqref="B7 B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -213,7 +219,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="37.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="23.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="9.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="37.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="37.83"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -234,13 +240,13 @@
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" s="0" t="s">
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>6</v>
       </c>
     </row>
@@ -248,10 +254,10 @@
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -259,10 +265,10 @@
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -270,10 +276,10 @@
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -281,10 +287,10 @@
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -292,10 +298,10 @@
       <c r="A7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -306,7 +312,18 @@
       <c r="B8" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -325,8 +342,10 @@
     <hyperlink ref="C6" r:id="rId11" display="Datasheet"/>
     <hyperlink ref="B7" r:id="rId12" display="DM3D-SF"/>
     <hyperlink ref="C7" r:id="rId13" display="Datasheet"/>
-    <hyperlink ref="B8" r:id="rId14" display="SN74LV1T34DCKRG4"/>
+    <hyperlink ref="B8" r:id="rId14" display="TBA-1-0510"/>
     <hyperlink ref="C8" r:id="rId15" display="Datasheet"/>
+    <hyperlink ref="B9" r:id="rId16" display="CD4504BEE4"/>
+    <hyperlink ref="C9" r:id="rId17" display="Datasheet"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -346,7 +365,7 @@
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="1" sqref="E11:E12 C1"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="2" sqref="B7 B11 C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -356,13 +375,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>